<commit_message>
fixes + videos in BO + discord in BO
</commit_message>
<xml_diff>
--- a/public/assets/BOs/Freyr.xlsx
+++ b/public/assets/BOs/Freyr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\doc\coding\DoD\DeitiesOfDeath\public\assets\BOs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03534585-166F-4DFB-9974-D48C64E2FC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACAC962-B78E-4D21-A395-6A6A38E13B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Archaic</t>
   </si>
@@ -434,13 +434,16 @@
   </si>
   <si>
     <t>Super Eco - By Mirez</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=FSVtc3pDO8w&amp;t=&amp;ab_channel=DeitiesofDeath</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -480,6 +483,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -563,10 +574,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -595,8 +607,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -875,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,6 +1081,11 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
@@ -1074,6 +1093,9 @@
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="A16:D16"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A19" r:id="rId1" tooltip="https://www.youtube.com/watch?v=FSVtc3pDO8w&amp;t=&amp;ab_channel=DeitiesofDeath" xr:uid="{EEA3F861-5A9F-41CE-9038-03C6C97C2F1F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>